<commit_message>
update UI: user's pages
</commit_message>
<xml_diff>
--- a/test/data.xlsx
+++ b/test/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="2" activeTab="9" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="add_service" sheetId="1" state="visible" r:id="rId1"/>
@@ -25,7 +25,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -34,12 +34,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <b val="1"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <b val="1"/>
       <sz val="11"/>
     </font>
@@ -60,27 +55,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -123,7 +103,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -131,11 +112,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -512,52 +489,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>min_price</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>max_price</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>category</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>image</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -1028,22 +1005,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -1065,7 +1042,6 @@
           <t>pass</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1083,7 +1059,6 @@
           <t>pass</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1105,37 +1080,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>fullname</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>username</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>password</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -1428,9 +1403,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="13.8"/>
   <cols>
-    <col width="14.69921875" customWidth="1" style="3" min="1" max="1"/>
-    <col width="15.8984375" customWidth="1" style="3" min="2" max="2"/>
-    <col width="20.59765625" customWidth="1" style="3" min="3" max="3"/>
+    <col width="14.69921875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="15.8984375" customWidth="1" style="1" min="2" max="2"/>
+    <col width="20.59765625" customWidth="1" style="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1545,72 +1520,72 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>friendly_name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>code_name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>email</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>phone</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>province</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>district</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>ward</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>street</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="K1" s="5" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>avatar</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -2710,52 +2685,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>item</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>note</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>province</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>district</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>ward</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>street</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -2922,37 +2897,37 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>item</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -3074,42 +3049,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>item</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>price</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -3151,6 +3126,7 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -3168,11 +3144,7 @@
           <t>Dịch vụ</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>50000</t>
@@ -3188,6 +3160,7 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3210,11 +3183,7 @@
           <t>2</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
           <t>price:invalid</t>
@@ -3225,6 +3194,7 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3262,6 +3232,7 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3299,6 +3270,7 @@
           <t>pass</t>
         </is>
       </c>
+      <c r="H6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3320,32 +3292,32 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>expiration_date</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>amount</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>
@@ -3555,52 +3527,52 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>order</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>payment</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>bank</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>card_number</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>card_holder</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>card_date</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>otp</t>
         </is>
       </c>
-      <c r="H1" s="5" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>expect</t>
         </is>
       </c>
-      <c r="I1" s="5" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>result</t>
         </is>
       </c>
-      <c r="J1" s="5" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>error</t>
         </is>

</xml_diff>